<commit_message>
[#11] Unresolved recommendation report
</commit_message>
<xml_diff>
--- a/xlsx/statuses.xlsx
+++ b/xlsx/statuses.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gohst\Documents\jgpersonal\CGJ\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisli/Projects/codeforsf/sf-civil-grand-jury/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67082EBF-5FB7-4E46-B1E0-B6EC9EB5C536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StatusCodeMapping" sheetId="1" r:id="rId1"/>
@@ -261,7 +262,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -576,23 +577,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="82.68359375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="76.89453125" customWidth="1"/>
-    <col min="3" max="3" width="64.3671875" customWidth="1"/>
-    <col min="5" max="5" width="96.1015625" customWidth="1"/>
-    <col min="6" max="6" width="77.26171875" customWidth="1"/>
+    <col min="1" max="1" width="82.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="76.83203125" customWidth="1"/>
+    <col min="3" max="3" width="64.33203125" customWidth="1"/>
+    <col min="5" max="5" width="96.1640625" customWidth="1"/>
+    <col min="6" max="6" width="77.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -606,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -620,7 +621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -634,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -648,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -662,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -676,7 +677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -684,7 +685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -692,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -700,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -708,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -716,7 +717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -724,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -732,7 +733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -740,7 +741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -748,7 +749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -756,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -764,7 +765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -772,7 +773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -780,7 +781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -788,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -796,7 +797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -804,7 +805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -812,7 +813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -820,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -828,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -836,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -844,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -852,7 +853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
@@ -860,7 +861,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>35</v>
       </c>
@@ -868,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -876,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>37</v>
       </c>
@@ -884,7 +885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>38</v>
       </c>
@@ -892,7 +893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -900,7 +901,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>40</v>
       </c>
@@ -908,7 +909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
@@ -916,7 +917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>3</v>
       </c>
@@ -924,7 +925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -932,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>43</v>
       </c>
@@ -940,7 +941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>44</v>
       </c>
@@ -948,7 +949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>45</v>
       </c>
@@ -956,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -964,7 +965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
@@ -972,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
@@ -980,7 +981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
@@ -988,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
@@ -996,7 +997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>50</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>53</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>55</v>
       </c>
@@ -1044,7 +1045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>56</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>58</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>60</v>
       </c>
@@ -1084,15 +1085,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>62</v>
       </c>
@@ -1100,7 +1101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>63</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
@@ -1116,7 +1117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
@@ -1124,7 +1125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>66</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
@@ -1140,7 +1141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>68</v>
       </c>
@@ -1148,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>69</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
@@ -1164,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
@@ -1180,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>73</v>
       </c>
@@ -1190,7 +1191,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Not Allowed by Penal Code" error="Only acceptable responses are the four listed in penal code 933.05(b)_x000a_" sqref="B1:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input Not Allowed by Penal Code" error="Only acceptable responses are the four listed in penal code 933.05(b)_x000a_" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$C$1:$C$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>